<commit_message>
Add 2 Endpoints In ProgramController GetProgramExcel Which Returns An Excel With All Data Of The Program UpdateProgramViaExcel Which Takes An Excel File And Update An Existing Program
</commit_message>
<xml_diff>
--- a/API/FOS/FOS.Doctor.API/ExcelTemplates/Program Template.xlsx
+++ b/API/FOS/FOS.Doctor.API/ExcelTemplates/Program Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Girguis\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA467E31-735D-4F7A-B64A-1E81413C3F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFFD39C-37AB-4FF9-9A80-F2B4DFB6B855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="بيانات البرنامج" sheetId="1" r:id="rId1"/>
@@ -320,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -356,14 +356,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5635,8 +5641,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="49" xr:uid="{EB33C9A1-8E37-40E7-8AF9-A9F7CA2A7757}" name="Table312144150" displayName="Table312144150" ref="A1:F68" totalsRowShown="0" headerRowDxfId="211" dataDxfId="210">
-  <autoFilter ref="A1:F68" xr:uid="{EB33C9A1-8E37-40E7-8AF9-A9F7CA2A7757}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="49" xr:uid="{EB33C9A1-8E37-40E7-8AF9-A9F7CA2A7757}" name="Table312144150" displayName="Table312144150" ref="A1:F2" totalsRowShown="0" headerRowDxfId="211" dataDxfId="210">
+  <autoFilter ref="A1:F2" xr:uid="{EB33C9A1-8E37-40E7-8AF9-A9F7CA2A7757}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{09F9B075-ADF5-4B27-8978-96EB67598A62}" name="كود المقرر" dataDxfId="209"/>
     <tableColumn id="2" xr3:uid="{3F90D0D7-1918-42F3-9601-2B53F509D4A8}" name="اسم المقرر" dataDxfId="208">
@@ -6357,7 +6363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A15:C15"/>
     </sheetView>
   </sheetViews>
@@ -6605,10 +6611,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1FE30A5-5EAF-407B-91C8-EC40DD522ADC}">
-  <dimension ref="A1:M68"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -6653,7 +6659,7 @@
     </row>
     <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="str">
-        <f t="shared" ref="B2:B33" si="0">IFERROR(VLOOKUP(A2,Course_Code_Name,2,0),"")</f>
+        <f t="shared" ref="B2:B34" si="0">IFERROR(VLOOKUP(A2,Course_Code_Name,2,0),"")</f>
         <v/>
       </c>
       <c r="G2" s="6"/>
@@ -6665,10 +6671,15 @@
       <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="A3" s="16"/>
+      <c r="B3" s="17" t="str">
+        <f>IFERROR(VLOOKUP(A3,Course_Code_Name,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="11" t="str">
         <f>'المقررات المتاحه'!H3</f>
         <v>ملاحظات
@@ -6950,13 +6961,13 @@
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="str">
-        <f t="shared" ref="B34:B65" si="1">IFERROR(VLOOKUP(A34,Course_Code_Name,2,0),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B35:B66" si="1">IFERROR(VLOOKUP(A35,Course_Code_Name,2,0),"")</f>
         <v/>
       </c>
     </row>
@@ -7142,18 +7153,24 @@
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" s="1" t="str">
-        <f t="shared" ref="B66:B97" si="2">IFERROR(VLOOKUP(A66,Course_Code_Name,2,0),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="B67:B69" si="2">IFERROR(VLOOKUP(A67,Course_Code_Name,2,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -7165,15 +7182,15 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B72" xr:uid="{06D2F85E-F711-4CFD-AF98-83ABF756AD64}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C72" xr:uid="{AE4F428A-2EC4-4C0C-82BC-B97DF72608ED}">
-      <formula1>"بدون متطلب, متطلب واحد,و,أو"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A68" xr:uid="{419ED6E6-B0C3-4110-ACF4-96E9A7468932}">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{419ED6E6-B0C3-4110-ACF4-96E9A7468932}">
       <formula1>Course_Code</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F68" xr:uid="{CA877BDA-13A6-4E53-A995-12118B1974AE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F2" xr:uid="{CA877BDA-13A6-4E53-A995-12118B1974AE}">
       <formula1>academic_Years</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B73" xr:uid="{06D2F85E-F711-4CFD-AF98-83ABF756AD64}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C73" xr:uid="{AE4F428A-2EC4-4C0C-82BC-B97DF72608ED}">
+      <formula1>"بدون متطلب, متطلب واحد,و,أو"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7188,43 +7205,43 @@
           <x14:formula1>
             <xm:f>'المقررات المتاحه'!$A1048301:A1048449</xm:f>
           </x14:formula1>
-          <xm:sqref>A1048481:A1048492</xm:sqref>
+          <xm:sqref>A1048482:A1048493</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2B0FE3E2-E897-4BD0-B18E-548226217296}">
           <x14:formula1>
             <xm:f>'المقررات المتاحه'!$A3:A151</xm:f>
           </x14:formula1>
-          <xm:sqref>A170:A1048479</xm:sqref>
+          <xm:sqref>A171:A1048480</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" xr:uid="{79C1B23E-6719-4F14-A013-4526DCF5AA69}">
           <x14:formula1>
             <xm:f>'المقررات المتاحه'!$A3:A50</xm:f>
           </x14:formula1>
-          <xm:sqref>A69:A77</xm:sqref>
+          <xm:sqref>A70:A78</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8FD209A8-8E87-47A7-A2D0-1EF43532E126}">
           <x14:formula1>
             <xm:f>'المقررات المتاحه'!$A3:A59</xm:f>
           </x14:formula1>
-          <xm:sqref>A78:A169</xm:sqref>
+          <xm:sqref>A79:A170</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9CD779BA-9005-45F3-A2FC-F6762F902D51}">
           <x14:formula1>
             <xm:f>'المقررات المتاحه'!$A1:A1048314</xm:f>
           </x14:formula1>
-          <xm:sqref>A1048494:A1048576</xm:sqref>
+          <xm:sqref>A1048495:A1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DE8BC8B-1790-44AC-94C7-F7B97CD62B0F}">
           <x14:formula1>
             <xm:f>'المقررات المتاحه'!$A1:A1048313</xm:f>
           </x14:formula1>
-          <xm:sqref>A1048493</xm:sqref>
+          <xm:sqref>A1048494</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" xr:uid="{27A37C5F-90D6-48DB-88AB-2CFD0E09CEAB}">
           <x14:formula1>
             <xm:f>'المقررات المتاحه'!$A1:A1048313</xm:f>
           </x14:formula1>
-          <xm:sqref>A1048480</xm:sqref>
+          <xm:sqref>A1048481</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7236,8 +7253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08FBFAE8-2DF1-43A5-B117-674CDBA1BB8E}">
   <dimension ref="A1:Q80"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A65" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -7252,22 +7269,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
       <c r="D1" s="1">
         <v>0</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:17" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -7366,11 +7383,11 @@
       <c r="Q5" s="11"/>
     </row>
     <row r="6" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="1">
         <v>0</v>
       </c>
@@ -7469,11 +7486,11 @@
       <c r="Q10" s="11"/>
     </row>
     <row r="11" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="1">
         <v>0</v>
       </c>
@@ -7557,11 +7574,11 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="1">
         <v>0</v>
       </c>
@@ -7612,11 +7629,11 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
       <c r="D21" s="1">
         <v>0</v>
       </c>
@@ -7660,11 +7677,11 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
       <c r="D26" s="1">
         <v>0</v>
       </c>
@@ -7708,11 +7725,11 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
       <c r="D31" s="1">
         <v>0</v>
       </c>
@@ -7756,11 +7773,11 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
       <c r="D36" s="1">
         <v>0</v>
       </c>
@@ -7804,11 +7821,11 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
       <c r="D41" s="1">
         <v>0</v>
       </c>
@@ -7852,11 +7869,11 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
       <c r="D46" s="1">
         <v>0</v>
       </c>
@@ -7900,11 +7917,11 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
       <c r="D51" s="1">
         <v>0</v>
       </c>
@@ -7948,11 +7965,11 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="14" t="s">
+      <c r="A56" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
       <c r="D56" s="1">
         <v>0</v>
       </c>
@@ -7996,11 +8013,11 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="14" t="s">
+      <c r="A61" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
+      <c r="B61" s="13"/>
+      <c r="C61" s="13"/>
       <c r="D61" s="1">
         <v>0</v>
       </c>
@@ -8044,11 +8061,11 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="14" t="s">
+      <c r="A66" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
       <c r="D66" s="1">
         <v>0</v>
       </c>
@@ -8092,11 +8109,11 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="14" t="s">
+      <c r="A71" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="13"/>
       <c r="D71" s="1">
         <v>0</v>
       </c>
@@ -8140,11 +8157,11 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="14" t="s">
+      <c r="A76" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B76" s="14"/>
-      <c r="C76" s="14"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
       <c r="D76" s="1">
         <v>0</v>
       </c>
@@ -8189,15 +8206,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A61:C61"/>
     <mergeCell ref="G1:L1"/>
     <mergeCell ref="G2:L13"/>
     <mergeCell ref="M2:Q13"/>
@@ -8208,6 +8216,15 @@
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A61:C61"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A5 A8:A10 A13:A15 A18:A20 A23:A25 A28:A30 A33:A35 A38:A40 A43:A45 A48:A50 A53:A55 A58:A60 A63:A65 A68:A70 A73:A75 A78:A80" xr:uid="{F078BC98-7875-4CC3-8B8B-714CB1F0BA16}">
@@ -8303,22 +8320,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
       <c r="D1" s="1">
         <v>0</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:17" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -8417,11 +8434,11 @@
       <c r="Q5" s="11"/>
     </row>
     <row r="6" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="1">
         <v>0</v>
       </c>
@@ -8520,11 +8537,11 @@
       <c r="Q10" s="11"/>
     </row>
     <row r="11" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="1">
         <v>0</v>
       </c>
@@ -8580,11 +8597,11 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="1">
         <v>0</v>
       </c>
@@ -8628,11 +8645,11 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
       <c r="D21" s="1">
         <v>0</v>
       </c>
@@ -8676,11 +8693,11 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
       <c r="D26" s="1">
         <v>0</v>
       </c>
@@ -8724,11 +8741,11 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
       <c r="D31" s="1">
         <v>0</v>
       </c>
@@ -8772,11 +8789,11 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
       <c r="D36" s="1">
         <v>0</v>
       </c>
@@ -8821,17 +8838,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="G1:L1"/>
-    <mergeCell ref="G2:L11"/>
-    <mergeCell ref="M2:Q11"/>
-    <mergeCell ref="A31:C31"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="G2:L11"/>
+    <mergeCell ref="M2:Q11"/>
+    <mergeCell ref="A31:C31"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="B38:B40 B3:B5 B8:B10 B13:B15 B33:B35 B18:B20 B28:B30 B23:B25" xr:uid="{D4CD4E0E-DB4C-4B40-B466-9FA722B2FF61}"/>

</xml_diff>